<commit_message>
All 50 Epoch complete
</commit_message>
<xml_diff>
--- a/Phase_I/End-Sem/50thresh_80epoch/test_results.xlsx
+++ b/Phase_I/End-Sem/50thresh_80epoch/test_results.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anind\Documents\Dissertation Codes\bar\drl_agent\testing_visualizations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Image name</t>
   </si>
@@ -137,13 +142,22 @@
   </si>
   <si>
     <t>Bad detections + STOP</t>
+  </si>
+  <si>
+    <t>IoU increase: 23</t>
+  </si>
+  <si>
+    <t>IoU decrease: 3</t>
+  </si>
+  <si>
+    <t>IoU average: 0.4615708595967316</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +194,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -226,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,9 +280,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -292,6 +315,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -467,14 +491,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:D34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -544,13 +570,13 @@
         <v>15</v>
       </c>
       <c r="J2">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="K2">
         <v>0.16</v>
       </c>
       <c r="L2">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M2">
         <v>10</v>
@@ -562,7 +588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -588,13 +614,13 @@
         <v>17</v>
       </c>
       <c r="J3">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="K3">
         <v>0.68</v>
       </c>
       <c r="L3">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="M3">
         <v>3</v>
@@ -606,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -650,7 +676,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -673,7 +699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -696,18 +722,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="C7">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D7">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -719,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -742,7 +768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -765,7 +791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -788,7 +814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -811,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -834,7 +860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -857,7 +883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -880,7 +906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -903,18 +929,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
       <c r="B16">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C16">
         <v>0.13</v>
       </c>
       <c r="D16">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -926,7 +952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -949,7 +975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -972,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -995,7 +1021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1018,18 +1044,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
       <c r="B21">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="C21">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="D21">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1041,12 +1067,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C22">
         <v>0.61</v>
@@ -1064,7 +1090,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1087,7 +1113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1110,21 +1136,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
       <c r="C25">
         <f>AVERAGE(C2:C24)</f>
-        <v>0</v>
+        <v>0.47347826086956524</v>
       </c>
       <c r="D25">
         <f>AVERAGE(D2:D24)</f>
-        <v>0</v>
+        <v>0.48956521739130426</v>
       </c>
       <c r="E25">
         <f>AVERAGE(E2:E24)</f>
-        <v>0</v>
+        <v>5.4782608695652177</v>
       </c>
       <c r="F25">
         <f>AVERAGE(F2:F24)</f>
@@ -1135,22 +1161,22 @@
       </c>
       <c r="K25">
         <f>AVERAGE(K2:K4)</f>
-        <v>0</v>
+        <v>0.3666666666666667</v>
       </c>
       <c r="L25">
         <f>AVERAGE(L2:L4)</f>
-        <v>0</v>
+        <v>0.4466666666666666</v>
       </c>
       <c r="M25">
         <f>AVERAGE(M2:M4)</f>
-        <v>0</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="N25">
         <f>AVERAGE(N2:N4)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1164,7 +1190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1178,7 +1204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1192,20 +1218,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="B30">
         <f>(SUM(C2:C24)-SUM(B2:B24))/23</f>
-        <v>0</v>
+        <v>5.6086956521739097E-2</v>
       </c>
       <c r="I30" t="s">
         <v>38</v>
       </c>
       <c r="J30">
         <f>(SUM(K2:K4)-SUM(J2:J4))/3</f>
-        <v>0</v>
+        <v>-6.3333333333333311E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>